<commit_message>
Added scaffold for Site and its related models: Address, Partner, and Audit. Changed the layout using Twitter Bootstrap.
</commit_message>
<xml_diff>
--- a/Tables.xlsx
+++ b/Tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
   </bookViews>
   <sheets>
     <sheet name="site" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="104">
   <si>
     <t>site_id</t>
   </si>
@@ -150,9 +150,6 @@
     <t>line</t>
   </si>
   <si>
-    <t>Share</t>
-  </si>
-  <si>
     <t>operator</t>
   </si>
   <si>
@@ -165,9 +162,6 @@
     <t>date</t>
   </si>
   <si>
-    <t>engineer</t>
-  </si>
-  <si>
     <t>this should be in proposal</t>
   </si>
   <si>
@@ -316,6 +310,24 @@
   </si>
   <si>
     <t>structure_height</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>decimal</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>Partner</t>
   </si>
 </sst>
 </file>
@@ -711,10 +723,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,7 +739,7 @@
     <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
@@ -740,150 +752,243 @@
         <v>32</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>44</v>
+        <v>103</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C2" t="s">
         <v>33</v>
       </c>
+      <c r="D2" t="s">
+        <v>98</v>
+      </c>
       <c r="E2" t="s">
         <v>8</v>
       </c>
+      <c r="F2" t="s">
+        <v>99</v>
+      </c>
       <c r="G2" t="s">
         <v>42</v>
       </c>
+      <c r="H2" t="s">
+        <v>98</v>
+      </c>
       <c r="I2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="J2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="s">
         <v>34</v>
       </c>
+      <c r="D3" t="s">
+        <v>98</v>
+      </c>
       <c r="E3" t="s">
         <v>9</v>
       </c>
+      <c r="F3" t="s">
+        <v>99</v>
+      </c>
       <c r="G3" t="s">
-        <v>45</v>
+        <v>44</v>
+      </c>
+      <c r="H3" t="s">
+        <v>98</v>
       </c>
       <c r="I3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="J3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C4" t="s">
         <v>35</v>
       </c>
+      <c r="D4" t="s">
+        <v>98</v>
+      </c>
       <c r="E4" t="s">
         <v>43</v>
       </c>
+      <c r="F4" t="s">
+        <v>98</v>
+      </c>
       <c r="G4" t="s">
         <v>33</v>
       </c>
+      <c r="H4" t="s">
+        <v>98</v>
+      </c>
       <c r="I4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="J4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C5" t="s">
         <v>36</v>
       </c>
+      <c r="D5" t="s">
+        <v>98</v>
+      </c>
       <c r="E5" t="s">
         <v>22</v>
       </c>
+      <c r="F5" t="s">
+        <v>98</v>
+      </c>
+      <c r="G5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" t="s">
+        <v>101</v>
+      </c>
       <c r="I5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C6" t="s">
         <v>37</v>
       </c>
+      <c r="D6" t="s">
+        <v>98</v>
+      </c>
       <c r="E6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+      <c r="F6" t="s">
+        <v>98</v>
+      </c>
+      <c r="I6" t="s">
+        <v>0</v>
+      </c>
+      <c r="J6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
       </c>
+      <c r="D7" t="s">
+        <v>98</v>
+      </c>
       <c r="E7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C8" t="s">
         <v>38</v>
       </c>
+      <c r="D8" t="s">
+        <v>98</v>
+      </c>
       <c r="E8" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="F8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C9" t="s">
         <v>13</v>
       </c>
+      <c r="D9" t="s">
+        <v>98</v>
+      </c>
       <c r="E9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="F9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C10" t="s">
+        <v>97</v>
+      </c>
+      <c r="D10" t="s">
         <v>99</v>
       </c>
       <c r="E10" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C11" t="s">
         <v>39</v>
       </c>
+      <c r="D11" t="s">
+        <v>99</v>
+      </c>
       <c r="E11" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>14</v>
       </c>
@@ -891,38 +996,59 @@
       <c r="C12" t="s">
         <v>40</v>
       </c>
+      <c r="D12" t="s">
+        <v>99</v>
+      </c>
       <c r="E12" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C13" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>98</v>
+      </c>
+      <c r="E13" t="s">
+        <v>0</v>
+      </c>
+      <c r="F13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C14" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C15" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>18</v>
       </c>
@@ -932,7 +1058,7 @@
         <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -940,7 +1066,7 @@
         <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -948,7 +1074,7 @@
         <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1034,13 +1160,13 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D1" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" s="10" t="s">
         <v>84</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1051,26 +1177,26 @@
         <v>33</v>
       </c>
       <c r="F2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F4" t="s">
         <v>33</v>
@@ -1078,162 +1204,162 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
@@ -1243,7 +1369,7 @@
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit before sector scaffold
</commit_message>
<xml_diff>
--- a/Tables.xlsx
+++ b/Tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
+    <workbookView xWindow="240" yWindow="285" windowWidth="14805" windowHeight="7830" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="site" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="107">
   <si>
     <t>site_id</t>
   </si>
@@ -328,6 +328,15 @@
   </si>
   <si>
     <t>Partner</t>
+  </si>
+  <si>
+    <t>design_status</t>
+  </si>
+  <si>
+    <t>cell</t>
+  </si>
+  <si>
+    <t>sector_id</t>
   </si>
 </sst>
 </file>
@@ -725,7 +734,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -1145,10 +1154,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1158,7 +1167,7 @@
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>53</v>
       </c>
@@ -1169,125 +1178,197 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="s">
         <v>33</v>
       </c>
+      <c r="E2" t="s">
+        <v>98</v>
+      </c>
       <c r="F2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>54</v>
       </c>
       <c r="D3" t="s">
-        <v>83</v>
+        <v>105</v>
+      </c>
+      <c r="E3" t="s">
+        <v>101</v>
       </c>
       <c r="F3" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>55</v>
       </c>
       <c r="D4" t="s">
-        <v>75</v>
+        <v>83</v>
+      </c>
+      <c r="E4" t="s">
+        <v>98</v>
       </c>
       <c r="F4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>56</v>
       </c>
       <c r="D5" t="s">
-        <v>63</v>
+        <v>75</v>
+      </c>
+      <c r="E5" t="s">
+        <v>98</v>
       </c>
       <c r="F5" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>57</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>86</v>
       </c>
+      <c r="E6" t="s">
+        <v>98</v>
+      </c>
       <c r="F6" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>58</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>87</v>
       </c>
+      <c r="E7" t="s">
+        <v>98</v>
+      </c>
       <c r="F7" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>59</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>88</v>
       </c>
+      <c r="E8" t="s">
+        <v>99</v>
+      </c>
       <c r="F8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>60</v>
       </c>
+      <c r="D9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" t="s">
+        <v>98</v>
+      </c>
       <c r="F9" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>61</v>
       </c>
+      <c r="D10" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>101</v>
+      </c>
       <c r="F10" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>104</v>
+      </c>
+      <c r="G11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>106</v>
+      </c>
+      <c r="G12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>67</v>
       </c>

</xml_diff>